<commit_message>
added manual confirmation of subject in test data
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylan/Desktop/Y4S1/BT4103/Capstone/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A912DF1A-4DFD-DD4A-8EF0-308548E60CAD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="22080" windowHeight="15060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="583">
   <si>
     <t>title</t>
   </si>
@@ -3398,12 +3404,15 @@
   <si>
     <t>N/A</t>
   </si>
+  <si>
+    <t>ground_confidence</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3435,7 +3444,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3458,6 +3467,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3466,12 +3486,15 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3479,6 +3502,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -3525,7 +3556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3557,9 +3588,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3591,6 +3640,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3766,14 +3833,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="H64" workbookViewId="0">
+      <selection activeCell="O87" sqref="O87"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="117.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="102.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3810,8 +3884,11 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" s="3" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3846,13 +3923,13 @@
         <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9019607843137255</v>
+        <v>0.90196078431372551</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -3893,7 +3970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>6</v>
       </c>
@@ -3934,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -3975,7 +4052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>12</v>
       </c>
@@ -4013,7 +4090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -4054,7 +4131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -4095,7 +4172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -4136,7 +4213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -4177,7 +4254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -4218,7 +4295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -4259,7 +4336,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -4300,7 +4377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4341,7 +4418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -4382,7 +4459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -4423,7 +4500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -4464,7 +4541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -4505,7 +4582,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -4546,7 +4623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -4587,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -4628,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -4669,7 +4746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>24</v>
       </c>
@@ -4710,7 +4787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -4748,7 +4825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -4789,7 +4866,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -4830,7 +4907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>9</v>
       </c>
@@ -4871,7 +4948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>12</v>
       </c>
@@ -4912,7 +4989,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -4953,7 +5030,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -4991,7 +5068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>6</v>
       </c>
@@ -5032,7 +5109,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>9</v>
       </c>
@@ -5073,7 +5150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -5114,7 +5191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -5155,7 +5232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>6</v>
       </c>
@@ -5196,7 +5273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>9</v>
       </c>
@@ -5237,7 +5314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>12</v>
       </c>
@@ -5278,7 +5355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>15</v>
       </c>
@@ -5310,7 +5387,7 @@
         <v>100</v>
       </c>
       <c r="K38">
-        <v>0.2222222222222222</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="L38">
         <v>0</v>
@@ -5319,7 +5396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>18</v>
       </c>
@@ -5360,7 +5437,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>0</v>
       </c>
@@ -5401,7 +5478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>3</v>
       </c>
@@ -5442,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>6</v>
       </c>
@@ -5483,7 +5560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>0</v>
       </c>
@@ -5515,7 +5592,7 @@
         <v>100</v>
       </c>
       <c r="K43">
-        <v>0.4285714285714285</v>
+        <v>0.42857142857142849</v>
       </c>
       <c r="L43">
         <v>1</v>
@@ -5524,7 +5601,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -5565,7 +5642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>6</v>
       </c>
@@ -5606,7 +5683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>9</v>
       </c>
@@ -5646,8 +5723,11 @@
       <c r="M46">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:13">
+      <c r="N46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>12</v>
       </c>
@@ -5687,8 +5767,11 @@
       <c r="M47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:13">
+      <c r="N47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>0</v>
       </c>
@@ -5728,8 +5811,11 @@
       <c r="M48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:13">
+      <c r="N48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -5769,8 +5855,11 @@
       <c r="M49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:13">
+      <c r="N49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>6</v>
       </c>
@@ -5807,8 +5896,11 @@
       <c r="M50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:13">
+      <c r="N50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>9</v>
       </c>
@@ -5848,8 +5940,11 @@
       <c r="M51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:13">
+      <c r="N51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>12</v>
       </c>
@@ -5886,8 +5981,11 @@
       <c r="M52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:13">
+      <c r="N52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>15</v>
       </c>
@@ -5927,8 +6025,11 @@
       <c r="M53">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:13">
+      <c r="N53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>6</v>
       </c>
@@ -5965,8 +6066,11 @@
       <c r="M54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:13">
+      <c r="N54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>9</v>
       </c>
@@ -6006,8 +6110,11 @@
       <c r="M55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:13">
+      <c r="N55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>15</v>
       </c>
@@ -6047,8 +6154,11 @@
       <c r="M56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:13">
+      <c r="N56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>18</v>
       </c>
@@ -6085,8 +6195,11 @@
       <c r="M57">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:13">
+      <c r="N57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>0</v>
       </c>
@@ -6126,8 +6239,11 @@
       <c r="M58">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:13">
+      <c r="N58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>3</v>
       </c>
@@ -6167,8 +6283,11 @@
       <c r="M59">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="N59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>6</v>
       </c>
@@ -6208,8 +6327,11 @@
       <c r="M60">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:13">
+      <c r="N60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>9</v>
       </c>
@@ -6249,8 +6371,11 @@
       <c r="M61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="N61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>12</v>
       </c>
@@ -6287,8 +6412,11 @@
       <c r="M62">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="N62">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>15</v>
       </c>
@@ -6328,8 +6456,11 @@
       <c r="M63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="N63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>18</v>
       </c>
@@ -6369,8 +6500,11 @@
       <c r="M64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:13">
+      <c r="N64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>21</v>
       </c>
@@ -6410,8 +6544,11 @@
       <c r="M65">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="N65">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>0</v>
       </c>
@@ -6448,8 +6585,11 @@
       <c r="M66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:13">
+      <c r="N66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>3</v>
       </c>
@@ -6489,8 +6629,11 @@
       <c r="M67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:13">
+      <c r="N67">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>0</v>
       </c>
@@ -6530,8 +6673,11 @@
       <c r="M68">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:13">
+      <c r="N68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>3</v>
       </c>
@@ -6571,8 +6717,11 @@
       <c r="M69">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:13">
+      <c r="N69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>6</v>
       </c>
@@ -6612,8 +6761,11 @@
       <c r="M70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:13">
+      <c r="N70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>9</v>
       </c>
@@ -6653,8 +6805,11 @@
       <c r="M71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:13">
+      <c r="N71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>12</v>
       </c>
@@ -6694,8 +6849,11 @@
       <c r="M72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:13">
+      <c r="N72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>15</v>
       </c>
@@ -6735,8 +6893,11 @@
       <c r="M73">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:13">
+      <c r="N73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>18</v>
       </c>
@@ -6776,8 +6937,11 @@
       <c r="M74">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:13">
+      <c r="N74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>0</v>
       </c>
@@ -6809,7 +6973,7 @@
         <v>100</v>
       </c>
       <c r="K75">
-        <v>0.6666666666666666</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="L75">
         <v>1</v>
@@ -6817,8 +6981,11 @@
       <c r="M75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:13">
+      <c r="N75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>3</v>
       </c>
@@ -6858,8 +7025,11 @@
       <c r="M76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:13">
+      <c r="N76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>6</v>
       </c>
@@ -6891,7 +7061,7 @@
         <v>100</v>
       </c>
       <c r="K77">
-        <v>0.7777777777777778</v>
+        <v>0.77777777777777779</v>
       </c>
       <c r="L77">
         <v>1</v>
@@ -6899,8 +7069,11 @@
       <c r="M77">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:13">
+      <c r="N77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>9</v>
       </c>
@@ -6932,7 +7105,7 @@
         <v>100</v>
       </c>
       <c r="K78">
-        <v>0.03571428571428571</v>
+        <v>3.5714285714285712E-2</v>
       </c>
       <c r="L78">
         <v>1</v>
@@ -6940,8 +7113,11 @@
       <c r="M78">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:13">
+      <c r="N78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>12</v>
       </c>
@@ -6981,8 +7157,11 @@
       <c r="M79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:13">
+      <c r="N79">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>15</v>
       </c>
@@ -7022,8 +7201,11 @@
       <c r="M80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:13">
+      <c r="N80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>0</v>
       </c>
@@ -7060,8 +7242,11 @@
       <c r="M81">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:13">
+      <c r="N81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>3</v>
       </c>
@@ -7101,8 +7286,11 @@
       <c r="M82">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:13">
+      <c r="N82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>6</v>
       </c>
@@ -7142,8 +7330,11 @@
       <c r="M83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:13">
+      <c r="N83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>0</v>
       </c>
@@ -7183,8 +7374,11 @@
       <c r="M84">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:13">
+      <c r="N84">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>3</v>
       </c>
@@ -7216,7 +7410,7 @@
         <v>100</v>
       </c>
       <c r="K85">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="L85">
         <v>0</v>
@@ -7224,8 +7418,11 @@
       <c r="M85">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:13">
+      <c r="N85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>0</v>
       </c>
@@ -7265,8 +7462,11 @@
       <c r="M86">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:13">
+      <c r="N86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>3</v>
       </c>
@@ -7306,8 +7506,11 @@
       <c r="M87">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:13">
+      <c r="N87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>6</v>
       </c>
@@ -7347,8 +7550,11 @@
       <c r="M88">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:13">
+      <c r="N88">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>9</v>
       </c>
@@ -7388,8 +7594,11 @@
       <c r="M89">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:13">
+      <c r="N89">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>12</v>
       </c>
@@ -7429,8 +7638,11 @@
       <c r="M90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:13">
+      <c r="N90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>0</v>
       </c>
@@ -7470,8 +7682,11 @@
       <c r="M91">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:13">
+      <c r="N91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>0</v>
       </c>
@@ -7508,8 +7723,11 @@
       <c r="M92">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:13">
+      <c r="N92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -7549,8 +7767,11 @@
       <c r="M93">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:13">
+      <c r="N93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>6</v>
       </c>
@@ -7590,102 +7811,105 @@
       <c r="M94">
         <v>0</v>
       </c>
+      <c r="N94">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12"/>
-    <hyperlink ref="F14" r:id="rId13"/>
-    <hyperlink ref="F15" r:id="rId14"/>
-    <hyperlink ref="F16" r:id="rId15"/>
-    <hyperlink ref="F17" r:id="rId16"/>
-    <hyperlink ref="F18" r:id="rId17"/>
-    <hyperlink ref="F19" r:id="rId18"/>
-    <hyperlink ref="F20" r:id="rId19"/>
-    <hyperlink ref="F21" r:id="rId20"/>
-    <hyperlink ref="F22" r:id="rId21"/>
-    <hyperlink ref="F23" r:id="rId22"/>
-    <hyperlink ref="F24" r:id="rId23"/>
-    <hyperlink ref="F25" r:id="rId24"/>
-    <hyperlink ref="F26" r:id="rId25"/>
-    <hyperlink ref="F27" r:id="rId26"/>
-    <hyperlink ref="F28" r:id="rId27"/>
-    <hyperlink ref="F29" r:id="rId28"/>
-    <hyperlink ref="F30" r:id="rId29"/>
-    <hyperlink ref="F31" r:id="rId30"/>
-    <hyperlink ref="F32" r:id="rId31"/>
-    <hyperlink ref="F33" r:id="rId32"/>
-    <hyperlink ref="F34" r:id="rId33"/>
-    <hyperlink ref="F35" r:id="rId34"/>
-    <hyperlink ref="F36" r:id="rId35"/>
-    <hyperlink ref="F37" r:id="rId36"/>
-    <hyperlink ref="F38" r:id="rId37"/>
-    <hyperlink ref="F39" r:id="rId38"/>
-    <hyperlink ref="F40" r:id="rId39"/>
-    <hyperlink ref="F41" r:id="rId40"/>
-    <hyperlink ref="F42" r:id="rId41"/>
-    <hyperlink ref="F43" r:id="rId42"/>
-    <hyperlink ref="F44" r:id="rId43"/>
-    <hyperlink ref="F45" r:id="rId44"/>
-    <hyperlink ref="F46" r:id="rId45"/>
-    <hyperlink ref="F47" r:id="rId46"/>
-    <hyperlink ref="F48" r:id="rId47"/>
-    <hyperlink ref="F49" r:id="rId48"/>
-    <hyperlink ref="F50" r:id="rId49"/>
-    <hyperlink ref="F51" r:id="rId50"/>
-    <hyperlink ref="F52" r:id="rId51"/>
-    <hyperlink ref="F53" r:id="rId52"/>
-    <hyperlink ref="F54" r:id="rId53"/>
-    <hyperlink ref="F55" r:id="rId54"/>
-    <hyperlink ref="F56" r:id="rId55"/>
-    <hyperlink ref="F57" r:id="rId56"/>
-    <hyperlink ref="F58" r:id="rId57"/>
-    <hyperlink ref="F59" r:id="rId58"/>
-    <hyperlink ref="F60" r:id="rId59"/>
-    <hyperlink ref="F61" r:id="rId60"/>
-    <hyperlink ref="F62" r:id="rId61"/>
-    <hyperlink ref="F63" r:id="rId62"/>
-    <hyperlink ref="F64" r:id="rId63"/>
-    <hyperlink ref="F65" r:id="rId64"/>
-    <hyperlink ref="F66" r:id="rId65"/>
-    <hyperlink ref="F67" r:id="rId66"/>
-    <hyperlink ref="F68" r:id="rId67"/>
-    <hyperlink ref="F69" r:id="rId68"/>
-    <hyperlink ref="F70" r:id="rId69"/>
-    <hyperlink ref="F71" r:id="rId70"/>
-    <hyperlink ref="F72" r:id="rId71"/>
-    <hyperlink ref="F73" r:id="rId72"/>
-    <hyperlink ref="F74" r:id="rId73"/>
-    <hyperlink ref="F75" r:id="rId74"/>
-    <hyperlink ref="F76" r:id="rId75"/>
-    <hyperlink ref="F77" r:id="rId76"/>
-    <hyperlink ref="F78" r:id="rId77"/>
-    <hyperlink ref="F79" r:id="rId78"/>
-    <hyperlink ref="F80" r:id="rId79"/>
-    <hyperlink ref="F81" r:id="rId80"/>
-    <hyperlink ref="F82" r:id="rId81"/>
-    <hyperlink ref="F83" r:id="rId82"/>
-    <hyperlink ref="F84" r:id="rId83"/>
-    <hyperlink ref="F85" r:id="rId84"/>
-    <hyperlink ref="F86" r:id="rId85"/>
-    <hyperlink ref="F87" r:id="rId86"/>
-    <hyperlink ref="F88" r:id="rId87"/>
-    <hyperlink ref="F89" r:id="rId88"/>
-    <hyperlink ref="F90" r:id="rId89"/>
-    <hyperlink ref="F91" r:id="rId90"/>
-    <hyperlink ref="F92" r:id="rId91"/>
-    <hyperlink ref="F93" r:id="rId92"/>
-    <hyperlink ref="F94" r:id="rId93"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="F23" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="F24" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="F25" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="F26" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="F27" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="F28" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="F29" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="F30" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="F31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="F32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="F33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="F34" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="F35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="F36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="F37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="F38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="F39" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="F40" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="F41" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="F42" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="F43" r:id="rId42" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="F44" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="F45" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="F46" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="F47" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="F48" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="F49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="F50" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="F51" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="F52" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="F53" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="F54" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="F55" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="F56" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="F57" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="F58" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="F59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="F60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="F61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="F62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="F63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="F64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="F65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="F66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="F67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="F68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="F69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="F70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="F71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="F72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="F73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="F74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="F75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="F76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="F77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="F78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="F79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="F80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="F81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="F82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="F83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="F84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="F85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="F86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="F87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="F88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="F89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="F90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="F91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="F92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="F93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="F94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added confidence score calculation
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Pictures\Y3S1\BT4013\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dylan/Desktop/Y4S1/BT4103/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13DBD3C9-6626-423F-8C86-894B36FB4BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5919D0B9-D101-DD47-A7AD-3A727088037B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="24540" windowHeight="16560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3958,20 +3958,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O94"/>
+  <dimension ref="A1:O353"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K176" sqref="K176:O353"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
       <c r="B1" s="9" t="s">
         <v>581</v>
@@ -4016,7 +4016,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <v>0</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -4110,7 +4110,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>6</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>12</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>15</v>
       </c>
@@ -4295,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>0</v>
       </c>
@@ -4342,7 +4342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -4389,7 +4389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>0</v>
       </c>
@@ -4436,7 +4436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>3</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>6</v>
       </c>
@@ -4530,7 +4530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>9</v>
       </c>
@@ -4577,7 +4577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>0</v>
       </c>
@@ -4671,7 +4671,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>3</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>6</v>
       </c>
@@ -4765,7 +4765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>9</v>
       </c>
@@ -4812,7 +4812,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>12</v>
       </c>
@@ -4859,7 +4859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -4906,7 +4906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>24</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>0</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>3</v>
       </c>
@@ -5138,7 +5138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>6</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>9</v>
       </c>
@@ -5232,7 +5232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>12</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>0</v>
       </c>
@@ -5326,7 +5326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3</v>
       </c>
@@ -5370,7 +5370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>6</v>
       </c>
@@ -5417,7 +5417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>9</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>0</v>
       </c>
@@ -5511,7 +5511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>3</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>6</v>
       </c>
@@ -5605,7 +5605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>9</v>
       </c>
@@ -5652,7 +5652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>12</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>15</v>
       </c>
@@ -5746,7 +5746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>18</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>0</v>
       </c>
@@ -5840,7 +5840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>3</v>
       </c>
@@ -5887,7 +5887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>6</v>
       </c>
@@ -5934,7 +5934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>0</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>3</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>6</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>9</v>
       </c>
@@ -6122,7 +6122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>12</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>0</v>
       </c>
@@ -6216,7 +6216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>3</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>6</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>9</v>
       </c>
@@ -6354,7 +6354,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>12</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>15</v>
       </c>
@@ -6445,7 +6445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>6</v>
       </c>
@@ -6489,7 +6489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>9</v>
       </c>
@@ -6536,7 +6536,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>15</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A57" s="10">
         <v>18</v>
       </c>
@@ -6627,7 +6627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A58" s="10">
         <v>0</v>
       </c>
@@ -6674,7 +6674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A59" s="10">
         <v>3</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A60" s="10">
         <v>6</v>
       </c>
@@ -6768,7 +6768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A61" s="10">
         <v>9</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A62" s="10">
         <v>12</v>
       </c>
@@ -6859,7 +6859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A63" s="10">
         <v>15</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>18</v>
       </c>
@@ -6953,7 +6953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>21</v>
       </c>
@@ -7000,7 +7000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>0</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>3</v>
       </c>
@@ -7091,7 +7091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>0</v>
       </c>
@@ -7138,7 +7138,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>3</v>
       </c>
@@ -7185,7 +7185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>6</v>
       </c>
@@ -7232,7 +7232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>9</v>
       </c>
@@ -7279,7 +7279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>12</v>
       </c>
@@ -7326,7 +7326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>15</v>
       </c>
@@ -7373,7 +7373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>18</v>
       </c>
@@ -7420,7 +7420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>0</v>
       </c>
@@ -7467,7 +7467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>3</v>
       </c>
@@ -7514,7 +7514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>6</v>
       </c>
@@ -7561,7 +7561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>9</v>
       </c>
@@ -7608,7 +7608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>12</v>
       </c>
@@ -7655,7 +7655,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>15</v>
       </c>
@@ -7702,7 +7702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>0</v>
       </c>
@@ -7746,7 +7746,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>3</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>6</v>
       </c>
@@ -7840,7 +7840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>0</v>
       </c>
@@ -7887,7 +7887,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>3</v>
       </c>
@@ -7934,7 +7934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>0</v>
       </c>
@@ -7981,7 +7981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>3</v>
       </c>
@@ -8028,7 +8028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>6</v>
       </c>
@@ -8075,7 +8075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>9</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>12</v>
       </c>
@@ -8169,7 +8169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>0</v>
       </c>
@@ -8216,7 +8216,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>0</v>
       </c>
@@ -8258,7 +8258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>3</v>
       </c>
@@ -8303,7 +8303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>6</v>
       </c>
@@ -8347,6 +8347,1917 @@
       <c r="O94" s="15">
         <v>1</v>
       </c>
+    </row>
+    <row r="95" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K95">
+        <v>0</v>
+      </c>
+      <c r="L95">
+        <v>0</v>
+      </c>
+      <c r="M95">
+        <v>0</v>
+      </c>
+      <c r="N95">
+        <v>0</v>
+      </c>
+      <c r="O95" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="K96">
+        <v>0</v>
+      </c>
+      <c r="L96">
+        <v>0</v>
+      </c>
+      <c r="M96">
+        <v>0</v>
+      </c>
+      <c r="N96">
+        <v>0</v>
+      </c>
+      <c r="O96" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K97">
+        <v>0</v>
+      </c>
+      <c r="L97">
+        <v>0</v>
+      </c>
+      <c r="M97">
+        <v>0</v>
+      </c>
+      <c r="N97">
+        <v>0</v>
+      </c>
+      <c r="O97" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K98">
+        <v>0</v>
+      </c>
+      <c r="L98">
+        <v>0</v>
+      </c>
+      <c r="M98">
+        <v>0</v>
+      </c>
+      <c r="N98">
+        <v>0</v>
+      </c>
+      <c r="O98" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K99">
+        <v>0</v>
+      </c>
+      <c r="L99">
+        <v>0</v>
+      </c>
+      <c r="M99">
+        <v>0</v>
+      </c>
+      <c r="N99">
+        <v>0</v>
+      </c>
+      <c r="O99" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K100">
+        <v>0</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100">
+        <v>0</v>
+      </c>
+      <c r="N100">
+        <v>0</v>
+      </c>
+      <c r="O100" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K101">
+        <v>0</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+      <c r="M101">
+        <v>0</v>
+      </c>
+      <c r="N101">
+        <v>0</v>
+      </c>
+      <c r="O101" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K102">
+        <v>0</v>
+      </c>
+      <c r="L102">
+        <v>0</v>
+      </c>
+      <c r="M102">
+        <v>0</v>
+      </c>
+      <c r="N102">
+        <v>0</v>
+      </c>
+      <c r="O102" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K103">
+        <v>0</v>
+      </c>
+      <c r="L103">
+        <v>0</v>
+      </c>
+      <c r="M103">
+        <v>0</v>
+      </c>
+      <c r="N103">
+        <v>0</v>
+      </c>
+      <c r="O103" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K104">
+        <v>0</v>
+      </c>
+      <c r="L104">
+        <v>0</v>
+      </c>
+      <c r="M104">
+        <v>0</v>
+      </c>
+      <c r="N104">
+        <v>0</v>
+      </c>
+      <c r="O104" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K105">
+        <v>0</v>
+      </c>
+      <c r="L105">
+        <v>0</v>
+      </c>
+      <c r="M105">
+        <v>0</v>
+      </c>
+      <c r="N105">
+        <v>0</v>
+      </c>
+      <c r="O105" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K106">
+        <v>0</v>
+      </c>
+      <c r="L106">
+        <v>0</v>
+      </c>
+      <c r="M106">
+        <v>0</v>
+      </c>
+      <c r="N106">
+        <v>0</v>
+      </c>
+      <c r="O106" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K107">
+        <v>0</v>
+      </c>
+      <c r="L107">
+        <v>0</v>
+      </c>
+      <c r="M107">
+        <v>0</v>
+      </c>
+      <c r="N107">
+        <v>0</v>
+      </c>
+      <c r="O107" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K108">
+        <v>0</v>
+      </c>
+      <c r="L108">
+        <v>0</v>
+      </c>
+      <c r="M108">
+        <v>0</v>
+      </c>
+      <c r="N108">
+        <v>0</v>
+      </c>
+      <c r="O108" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K109">
+        <v>0</v>
+      </c>
+      <c r="L109">
+        <v>0</v>
+      </c>
+      <c r="M109">
+        <v>0</v>
+      </c>
+      <c r="N109">
+        <v>0</v>
+      </c>
+      <c r="O109" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K110">
+        <v>0</v>
+      </c>
+      <c r="L110">
+        <v>0</v>
+      </c>
+      <c r="M110">
+        <v>0</v>
+      </c>
+      <c r="N110">
+        <v>0</v>
+      </c>
+      <c r="O110" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K111">
+        <v>0</v>
+      </c>
+      <c r="L111">
+        <v>0</v>
+      </c>
+      <c r="M111">
+        <v>0</v>
+      </c>
+      <c r="N111">
+        <v>0</v>
+      </c>
+      <c r="O111" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K112">
+        <v>0</v>
+      </c>
+      <c r="L112">
+        <v>0</v>
+      </c>
+      <c r="M112">
+        <v>0</v>
+      </c>
+      <c r="N112">
+        <v>0</v>
+      </c>
+      <c r="O112" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K113">
+        <v>0</v>
+      </c>
+      <c r="L113">
+        <v>0</v>
+      </c>
+      <c r="M113">
+        <v>0</v>
+      </c>
+      <c r="N113">
+        <v>0</v>
+      </c>
+      <c r="O113" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K114">
+        <v>0</v>
+      </c>
+      <c r="L114">
+        <v>0</v>
+      </c>
+      <c r="M114">
+        <v>0</v>
+      </c>
+      <c r="N114">
+        <v>0</v>
+      </c>
+      <c r="O114" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K115">
+        <v>0</v>
+      </c>
+      <c r="L115">
+        <v>0</v>
+      </c>
+      <c r="M115">
+        <v>0</v>
+      </c>
+      <c r="N115">
+        <v>0</v>
+      </c>
+      <c r="O115" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K116">
+        <v>0</v>
+      </c>
+      <c r="L116">
+        <v>0</v>
+      </c>
+      <c r="M116">
+        <v>0</v>
+      </c>
+      <c r="N116">
+        <v>0</v>
+      </c>
+      <c r="O116" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K117">
+        <v>0</v>
+      </c>
+      <c r="L117">
+        <v>0</v>
+      </c>
+      <c r="M117">
+        <v>0</v>
+      </c>
+      <c r="N117">
+        <v>0</v>
+      </c>
+      <c r="O117" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K118">
+        <v>0</v>
+      </c>
+      <c r="L118">
+        <v>0</v>
+      </c>
+      <c r="M118">
+        <v>0</v>
+      </c>
+      <c r="N118">
+        <v>0</v>
+      </c>
+      <c r="O118" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K119">
+        <v>0</v>
+      </c>
+      <c r="L119">
+        <v>0</v>
+      </c>
+      <c r="M119">
+        <v>0</v>
+      </c>
+      <c r="N119">
+        <v>0</v>
+      </c>
+      <c r="O119" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K120">
+        <v>0</v>
+      </c>
+      <c r="L120">
+        <v>0</v>
+      </c>
+      <c r="M120">
+        <v>0</v>
+      </c>
+      <c r="N120">
+        <v>0</v>
+      </c>
+      <c r="O120" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K121">
+        <v>0</v>
+      </c>
+      <c r="L121">
+        <v>0</v>
+      </c>
+      <c r="M121">
+        <v>0</v>
+      </c>
+      <c r="N121">
+        <v>0</v>
+      </c>
+      <c r="O121" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K122">
+        <v>0</v>
+      </c>
+      <c r="L122">
+        <v>0</v>
+      </c>
+      <c r="M122">
+        <v>0</v>
+      </c>
+      <c r="N122">
+        <v>0</v>
+      </c>
+      <c r="O122" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K123">
+        <v>0</v>
+      </c>
+      <c r="L123">
+        <v>0</v>
+      </c>
+      <c r="M123">
+        <v>0</v>
+      </c>
+      <c r="N123">
+        <v>0</v>
+      </c>
+      <c r="O123" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K124">
+        <v>0</v>
+      </c>
+      <c r="L124">
+        <v>0</v>
+      </c>
+      <c r="M124">
+        <v>0</v>
+      </c>
+      <c r="N124">
+        <v>0</v>
+      </c>
+      <c r="O124" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="125" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K125">
+        <v>0</v>
+      </c>
+      <c r="L125">
+        <v>0</v>
+      </c>
+      <c r="M125">
+        <v>0</v>
+      </c>
+      <c r="N125">
+        <v>0</v>
+      </c>
+      <c r="O125" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K126">
+        <v>0</v>
+      </c>
+      <c r="L126">
+        <v>0</v>
+      </c>
+      <c r="M126">
+        <v>0</v>
+      </c>
+      <c r="N126">
+        <v>0</v>
+      </c>
+      <c r="O126" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K127">
+        <v>0</v>
+      </c>
+      <c r="L127">
+        <v>0</v>
+      </c>
+      <c r="M127">
+        <v>0</v>
+      </c>
+      <c r="N127">
+        <v>0</v>
+      </c>
+      <c r="O127" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K128">
+        <v>0</v>
+      </c>
+      <c r="L128">
+        <v>0</v>
+      </c>
+      <c r="M128">
+        <v>0</v>
+      </c>
+      <c r="N128">
+        <v>0</v>
+      </c>
+      <c r="O128" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K129">
+        <v>0</v>
+      </c>
+      <c r="L129">
+        <v>0</v>
+      </c>
+      <c r="M129">
+        <v>0</v>
+      </c>
+      <c r="N129">
+        <v>0</v>
+      </c>
+      <c r="O129" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K130">
+        <v>0</v>
+      </c>
+      <c r="L130">
+        <v>0</v>
+      </c>
+      <c r="M130">
+        <v>0</v>
+      </c>
+      <c r="N130">
+        <v>0</v>
+      </c>
+      <c r="O130" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K131">
+        <v>0</v>
+      </c>
+      <c r="L131">
+        <v>0</v>
+      </c>
+      <c r="M131">
+        <v>0</v>
+      </c>
+      <c r="N131">
+        <v>0</v>
+      </c>
+      <c r="O131" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K132">
+        <v>0</v>
+      </c>
+      <c r="L132">
+        <v>0</v>
+      </c>
+      <c r="M132">
+        <v>0</v>
+      </c>
+      <c r="N132">
+        <v>0</v>
+      </c>
+      <c r="O132" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K133">
+        <v>0</v>
+      </c>
+      <c r="L133">
+        <v>0</v>
+      </c>
+      <c r="M133">
+        <v>0</v>
+      </c>
+      <c r="N133">
+        <v>0</v>
+      </c>
+      <c r="O133" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K134">
+        <v>0</v>
+      </c>
+      <c r="L134">
+        <v>0</v>
+      </c>
+      <c r="M134">
+        <v>0</v>
+      </c>
+      <c r="N134">
+        <v>0</v>
+      </c>
+      <c r="O134" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="135" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K135">
+        <v>0</v>
+      </c>
+      <c r="L135">
+        <v>0</v>
+      </c>
+      <c r="M135">
+        <v>0</v>
+      </c>
+      <c r="N135">
+        <v>0</v>
+      </c>
+      <c r="O135" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K136">
+        <v>0</v>
+      </c>
+      <c r="L136">
+        <v>0</v>
+      </c>
+      <c r="M136">
+        <v>0</v>
+      </c>
+      <c r="N136">
+        <v>0</v>
+      </c>
+      <c r="O136" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K137">
+        <v>0</v>
+      </c>
+      <c r="L137">
+        <v>0</v>
+      </c>
+      <c r="M137">
+        <v>0</v>
+      </c>
+      <c r="N137">
+        <v>0</v>
+      </c>
+      <c r="O137" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K138">
+        <v>0</v>
+      </c>
+      <c r="L138">
+        <v>0</v>
+      </c>
+      <c r="M138">
+        <v>0</v>
+      </c>
+      <c r="N138">
+        <v>0</v>
+      </c>
+      <c r="O138" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K139">
+        <v>0</v>
+      </c>
+      <c r="L139">
+        <v>0</v>
+      </c>
+      <c r="M139">
+        <v>0</v>
+      </c>
+      <c r="N139">
+        <v>0</v>
+      </c>
+      <c r="O139" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K140">
+        <v>0</v>
+      </c>
+      <c r="L140">
+        <v>0</v>
+      </c>
+      <c r="M140">
+        <v>0</v>
+      </c>
+      <c r="N140">
+        <v>0</v>
+      </c>
+      <c r="O140" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K141">
+        <v>0</v>
+      </c>
+      <c r="L141">
+        <v>0</v>
+      </c>
+      <c r="M141">
+        <v>0</v>
+      </c>
+      <c r="N141">
+        <v>0</v>
+      </c>
+      <c r="O141" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K142">
+        <v>0</v>
+      </c>
+      <c r="L142">
+        <v>0</v>
+      </c>
+      <c r="M142">
+        <v>0</v>
+      </c>
+      <c r="N142">
+        <v>0</v>
+      </c>
+      <c r="O142" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K143">
+        <v>0</v>
+      </c>
+      <c r="L143">
+        <v>0</v>
+      </c>
+      <c r="M143">
+        <v>0</v>
+      </c>
+      <c r="N143">
+        <v>0</v>
+      </c>
+      <c r="O143" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K144">
+        <v>0</v>
+      </c>
+      <c r="L144">
+        <v>0</v>
+      </c>
+      <c r="M144">
+        <v>0</v>
+      </c>
+      <c r="N144">
+        <v>0</v>
+      </c>
+      <c r="O144" s="15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K145">
+        <v>100</v>
+      </c>
+      <c r="L145">
+        <v>1</v>
+      </c>
+      <c r="M145">
+        <v>1</v>
+      </c>
+      <c r="N145">
+        <v>1</v>
+      </c>
+      <c r="O145" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K146">
+        <v>100</v>
+      </c>
+      <c r="L146">
+        <v>1</v>
+      </c>
+      <c r="M146">
+        <v>1</v>
+      </c>
+      <c r="N146">
+        <v>1</v>
+      </c>
+      <c r="O146" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K147">
+        <v>100</v>
+      </c>
+      <c r="L147">
+        <v>1</v>
+      </c>
+      <c r="M147">
+        <v>1</v>
+      </c>
+      <c r="N147">
+        <v>1</v>
+      </c>
+      <c r="O147" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K148">
+        <v>100</v>
+      </c>
+      <c r="L148">
+        <v>1</v>
+      </c>
+      <c r="M148">
+        <v>1</v>
+      </c>
+      <c r="N148">
+        <v>1</v>
+      </c>
+      <c r="O148" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K149">
+        <v>100</v>
+      </c>
+      <c r="L149">
+        <v>1</v>
+      </c>
+      <c r="M149">
+        <v>1</v>
+      </c>
+      <c r="N149">
+        <v>1</v>
+      </c>
+      <c r="O149" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K150">
+        <v>100</v>
+      </c>
+      <c r="L150">
+        <v>1</v>
+      </c>
+      <c r="M150">
+        <v>1</v>
+      </c>
+      <c r="N150">
+        <v>1</v>
+      </c>
+      <c r="O150" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K151">
+        <v>100</v>
+      </c>
+      <c r="L151">
+        <v>1</v>
+      </c>
+      <c r="M151">
+        <v>1</v>
+      </c>
+      <c r="N151">
+        <v>1</v>
+      </c>
+      <c r="O151" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K152">
+        <v>100</v>
+      </c>
+      <c r="L152">
+        <v>1</v>
+      </c>
+      <c r="M152">
+        <v>1</v>
+      </c>
+      <c r="N152">
+        <v>1</v>
+      </c>
+      <c r="O152" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K153">
+        <v>100</v>
+      </c>
+      <c r="L153">
+        <v>1</v>
+      </c>
+      <c r="M153">
+        <v>1</v>
+      </c>
+      <c r="N153">
+        <v>1</v>
+      </c>
+      <c r="O153" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="154" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K154">
+        <v>100</v>
+      </c>
+      <c r="L154">
+        <v>1</v>
+      </c>
+      <c r="M154">
+        <v>1</v>
+      </c>
+      <c r="N154">
+        <v>1</v>
+      </c>
+      <c r="O154" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K155">
+        <v>100</v>
+      </c>
+      <c r="L155">
+        <v>1</v>
+      </c>
+      <c r="M155">
+        <v>1</v>
+      </c>
+      <c r="N155">
+        <v>1</v>
+      </c>
+      <c r="O155" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K156">
+        <v>100</v>
+      </c>
+      <c r="L156">
+        <v>1</v>
+      </c>
+      <c r="M156">
+        <v>1</v>
+      </c>
+      <c r="N156">
+        <v>1</v>
+      </c>
+      <c r="O156" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K157">
+        <v>100</v>
+      </c>
+      <c r="L157">
+        <v>1</v>
+      </c>
+      <c r="M157">
+        <v>1</v>
+      </c>
+      <c r="N157">
+        <v>1</v>
+      </c>
+      <c r="O157" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K158">
+        <v>100</v>
+      </c>
+      <c r="L158">
+        <v>1</v>
+      </c>
+      <c r="M158">
+        <v>1</v>
+      </c>
+      <c r="N158">
+        <v>1</v>
+      </c>
+      <c r="O158" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K159">
+        <v>100</v>
+      </c>
+      <c r="L159">
+        <v>1</v>
+      </c>
+      <c r="M159">
+        <v>1</v>
+      </c>
+      <c r="N159">
+        <v>1</v>
+      </c>
+      <c r="O159" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K160">
+        <v>100</v>
+      </c>
+      <c r="L160">
+        <v>1</v>
+      </c>
+      <c r="M160">
+        <v>1</v>
+      </c>
+      <c r="N160">
+        <v>1</v>
+      </c>
+      <c r="O160" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K161">
+        <v>100</v>
+      </c>
+      <c r="L161">
+        <v>1</v>
+      </c>
+      <c r="M161">
+        <v>1</v>
+      </c>
+      <c r="N161">
+        <v>1</v>
+      </c>
+      <c r="O161" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K162">
+        <v>100</v>
+      </c>
+      <c r="L162">
+        <v>1</v>
+      </c>
+      <c r="M162">
+        <v>1</v>
+      </c>
+      <c r="N162">
+        <v>1</v>
+      </c>
+      <c r="O162" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K163">
+        <v>100</v>
+      </c>
+      <c r="L163">
+        <v>1</v>
+      </c>
+      <c r="M163">
+        <v>1</v>
+      </c>
+      <c r="N163">
+        <v>1</v>
+      </c>
+      <c r="O163" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K164">
+        <v>100</v>
+      </c>
+      <c r="L164">
+        <v>1</v>
+      </c>
+      <c r="M164">
+        <v>1</v>
+      </c>
+      <c r="N164">
+        <v>1</v>
+      </c>
+      <c r="O164" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K165">
+        <v>100</v>
+      </c>
+      <c r="L165">
+        <v>1</v>
+      </c>
+      <c r="M165">
+        <v>1</v>
+      </c>
+      <c r="N165">
+        <v>1</v>
+      </c>
+      <c r="O165" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K166">
+        <v>100</v>
+      </c>
+      <c r="L166">
+        <v>1</v>
+      </c>
+      <c r="M166">
+        <v>1</v>
+      </c>
+      <c r="N166">
+        <v>1</v>
+      </c>
+      <c r="O166" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K167">
+        <v>100</v>
+      </c>
+      <c r="L167">
+        <v>1</v>
+      </c>
+      <c r="M167">
+        <v>1</v>
+      </c>
+      <c r="N167">
+        <v>1</v>
+      </c>
+      <c r="O167" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K168">
+        <v>100</v>
+      </c>
+      <c r="L168">
+        <v>1</v>
+      </c>
+      <c r="M168">
+        <v>1</v>
+      </c>
+      <c r="N168">
+        <v>1</v>
+      </c>
+      <c r="O168" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K169">
+        <v>100</v>
+      </c>
+      <c r="L169">
+        <v>1</v>
+      </c>
+      <c r="M169">
+        <v>1</v>
+      </c>
+      <c r="N169">
+        <v>1</v>
+      </c>
+      <c r="O169" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K170">
+        <v>100</v>
+      </c>
+      <c r="L170">
+        <v>1</v>
+      </c>
+      <c r="M170">
+        <v>1</v>
+      </c>
+      <c r="N170">
+        <v>1</v>
+      </c>
+      <c r="O170" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K171">
+        <v>100</v>
+      </c>
+      <c r="L171">
+        <v>1</v>
+      </c>
+      <c r="M171">
+        <v>1</v>
+      </c>
+      <c r="N171">
+        <v>1</v>
+      </c>
+      <c r="O171" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K172">
+        <v>100</v>
+      </c>
+      <c r="L172">
+        <v>1</v>
+      </c>
+      <c r="M172">
+        <v>1</v>
+      </c>
+      <c r="N172">
+        <v>1</v>
+      </c>
+      <c r="O172" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K173">
+        <v>100</v>
+      </c>
+      <c r="L173">
+        <v>1</v>
+      </c>
+      <c r="M173">
+        <v>1</v>
+      </c>
+      <c r="N173">
+        <v>1</v>
+      </c>
+      <c r="O173" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K174">
+        <v>100</v>
+      </c>
+      <c r="L174">
+        <v>1</v>
+      </c>
+      <c r="M174">
+        <v>1</v>
+      </c>
+      <c r="N174">
+        <v>1</v>
+      </c>
+      <c r="O174" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="K175">
+        <v>100</v>
+      </c>
+      <c r="L175">
+        <v>1</v>
+      </c>
+      <c r="M175">
+        <v>1</v>
+      </c>
+      <c r="N175">
+        <v>1</v>
+      </c>
+      <c r="O175" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="11:15" x14ac:dyDescent="0.2">
+      <c r="O176" s="15"/>
+    </row>
+    <row r="177" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O177" s="15"/>
+    </row>
+    <row r="178" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O178" s="15"/>
+    </row>
+    <row r="179" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O179" s="15"/>
+    </row>
+    <row r="180" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O180" s="15"/>
+    </row>
+    <row r="181" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O181" s="15"/>
+    </row>
+    <row r="182" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O182" s="15"/>
+    </row>
+    <row r="183" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O183" s="15"/>
+    </row>
+    <row r="184" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O184" s="15"/>
+    </row>
+    <row r="185" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O185" s="15"/>
+    </row>
+    <row r="186" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O186" s="15"/>
+    </row>
+    <row r="187" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O187" s="15"/>
+    </row>
+    <row r="188" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O188" s="15"/>
+    </row>
+    <row r="189" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O189" s="15"/>
+    </row>
+    <row r="190" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O190" s="15"/>
+    </row>
+    <row r="191" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O191" s="15"/>
+    </row>
+    <row r="192" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O192" s="15"/>
+    </row>
+    <row r="193" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O193" s="15"/>
+    </row>
+    <row r="194" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O194" s="15"/>
+    </row>
+    <row r="195" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O195" s="15"/>
+    </row>
+    <row r="196" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O196" s="15"/>
+    </row>
+    <row r="197" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O197" s="15"/>
+    </row>
+    <row r="198" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O198" s="15"/>
+    </row>
+    <row r="199" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O199" s="15"/>
+    </row>
+    <row r="200" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O200" s="15"/>
+    </row>
+    <row r="201" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O201" s="15"/>
+    </row>
+    <row r="202" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O202" s="15"/>
+    </row>
+    <row r="203" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O203" s="15"/>
+    </row>
+    <row r="204" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O204" s="15"/>
+    </row>
+    <row r="205" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O205" s="15"/>
+    </row>
+    <row r="206" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O206" s="15"/>
+    </row>
+    <row r="207" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O207" s="15"/>
+    </row>
+    <row r="208" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O208" s="15"/>
+    </row>
+    <row r="209" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O209" s="15"/>
+    </row>
+    <row r="210" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O210" s="15"/>
+    </row>
+    <row r="211" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O211" s="15"/>
+    </row>
+    <row r="212" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O212" s="15"/>
+    </row>
+    <row r="213" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O213" s="15"/>
+    </row>
+    <row r="214" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O214" s="15"/>
+    </row>
+    <row r="215" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O215" s="15"/>
+    </row>
+    <row r="216" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O216" s="15"/>
+    </row>
+    <row r="217" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O217" s="15"/>
+    </row>
+    <row r="218" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O218" s="15"/>
+    </row>
+    <row r="219" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O219" s="15"/>
+    </row>
+    <row r="220" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O220" s="15"/>
+    </row>
+    <row r="221" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O221" s="15"/>
+    </row>
+    <row r="222" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O222" s="15"/>
+    </row>
+    <row r="223" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O223" s="15"/>
+    </row>
+    <row r="224" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O224" s="15"/>
+    </row>
+    <row r="225" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O225" s="15"/>
+    </row>
+    <row r="226" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O226" s="15"/>
+    </row>
+    <row r="227" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O227" s="15"/>
+    </row>
+    <row r="228" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O228" s="15"/>
+    </row>
+    <row r="229" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O229" s="15"/>
+    </row>
+    <row r="230" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O230" s="15"/>
+    </row>
+    <row r="231" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O231" s="15"/>
+    </row>
+    <row r="232" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O232" s="15"/>
+    </row>
+    <row r="233" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O233" s="15"/>
+    </row>
+    <row r="234" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O234" s="15"/>
+    </row>
+    <row r="235" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O235" s="15"/>
+    </row>
+    <row r="236" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O236" s="15"/>
+    </row>
+    <row r="237" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O237" s="15"/>
+    </row>
+    <row r="238" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O238" s="15"/>
+    </row>
+    <row r="239" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O239" s="15"/>
+    </row>
+    <row r="240" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O240" s="15"/>
+    </row>
+    <row r="241" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O241" s="15"/>
+    </row>
+    <row r="242" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O242" s="15"/>
+    </row>
+    <row r="243" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O243" s="15"/>
+    </row>
+    <row r="244" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O244" s="15"/>
+    </row>
+    <row r="245" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O245" s="15"/>
+    </row>
+    <row r="246" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O246" s="15"/>
+    </row>
+    <row r="247" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O247" s="15"/>
+    </row>
+    <row r="248" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O248" s="15"/>
+    </row>
+    <row r="249" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O249" s="15"/>
+    </row>
+    <row r="250" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O250" s="15"/>
+    </row>
+    <row r="251" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O251" s="15"/>
+    </row>
+    <row r="252" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O252" s="15"/>
+    </row>
+    <row r="253" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O253" s="15"/>
+    </row>
+    <row r="254" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O254" s="15"/>
+    </row>
+    <row r="255" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O255" s="15"/>
+    </row>
+    <row r="256" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O256" s="15"/>
+    </row>
+    <row r="257" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O257" s="15"/>
+    </row>
+    <row r="258" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O258" s="15"/>
+    </row>
+    <row r="259" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O259" s="15"/>
+    </row>
+    <row r="260" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O260" s="15"/>
+    </row>
+    <row r="261" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O261" s="15"/>
+    </row>
+    <row r="262" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O262" s="15"/>
+    </row>
+    <row r="263" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O263" s="15"/>
+    </row>
+    <row r="264" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O264" s="15"/>
+    </row>
+    <row r="265" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O265" s="15"/>
+    </row>
+    <row r="266" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O266" s="15"/>
+    </row>
+    <row r="267" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O267" s="15"/>
+    </row>
+    <row r="268" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O268" s="15"/>
+    </row>
+    <row r="269" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O269" s="15"/>
+    </row>
+    <row r="270" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O270" s="15"/>
+    </row>
+    <row r="271" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O271" s="15"/>
+    </row>
+    <row r="272" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O272" s="15"/>
+    </row>
+    <row r="273" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O273" s="15"/>
+    </row>
+    <row r="274" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O274" s="15"/>
+    </row>
+    <row r="275" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O275" s="15"/>
+    </row>
+    <row r="276" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O276" s="15"/>
+    </row>
+    <row r="277" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O277" s="15"/>
+    </row>
+    <row r="278" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O278" s="15"/>
+    </row>
+    <row r="279" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O279" s="15"/>
+    </row>
+    <row r="280" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O280" s="15"/>
+    </row>
+    <row r="281" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O281" s="15"/>
+    </row>
+    <row r="282" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O282" s="15"/>
+    </row>
+    <row r="283" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O283" s="15"/>
+    </row>
+    <row r="284" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O284" s="15"/>
+    </row>
+    <row r="285" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O285" s="15"/>
+    </row>
+    <row r="286" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O286" s="15"/>
+    </row>
+    <row r="287" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O287" s="15"/>
+    </row>
+    <row r="288" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O288" s="15"/>
+    </row>
+    <row r="289" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O289" s="15"/>
+    </row>
+    <row r="290" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O290" s="15"/>
+    </row>
+    <row r="291" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O291" s="15"/>
+    </row>
+    <row r="292" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O292" s="15"/>
+    </row>
+    <row r="293" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O293" s="15"/>
+    </row>
+    <row r="294" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O294" s="15"/>
+    </row>
+    <row r="295" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O295" s="15"/>
+    </row>
+    <row r="296" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O296" s="15"/>
+    </row>
+    <row r="297" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O297" s="15"/>
+    </row>
+    <row r="298" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O298" s="15"/>
+    </row>
+    <row r="299" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O299" s="15"/>
+    </row>
+    <row r="300" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O300" s="15"/>
+    </row>
+    <row r="301" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O301" s="15"/>
+    </row>
+    <row r="302" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O302" s="15"/>
+    </row>
+    <row r="303" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O303" s="15"/>
+    </row>
+    <row r="304" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O304" s="15"/>
+    </row>
+    <row r="305" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O305" s="15"/>
+    </row>
+    <row r="306" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O306" s="15"/>
+    </row>
+    <row r="307" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O307" s="15"/>
+    </row>
+    <row r="308" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O308" s="15"/>
+    </row>
+    <row r="309" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O309" s="15"/>
+    </row>
+    <row r="310" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O310" s="15"/>
+    </row>
+    <row r="311" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O311" s="15"/>
+    </row>
+    <row r="312" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O312" s="15"/>
+    </row>
+    <row r="313" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O313" s="15"/>
+    </row>
+    <row r="314" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O314" s="15"/>
+    </row>
+    <row r="315" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O315" s="15"/>
+    </row>
+    <row r="316" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O316" s="15"/>
+    </row>
+    <row r="317" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O317" s="15"/>
+    </row>
+    <row r="318" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O318" s="15"/>
+    </row>
+    <row r="319" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O319" s="15"/>
+    </row>
+    <row r="320" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O320" s="15"/>
+    </row>
+    <row r="321" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O321" s="15"/>
+    </row>
+    <row r="322" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O322" s="15"/>
+    </row>
+    <row r="323" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O323" s="15"/>
+    </row>
+    <row r="324" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O324" s="15"/>
+    </row>
+    <row r="325" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O325" s="15"/>
+    </row>
+    <row r="326" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O326" s="15"/>
+    </row>
+    <row r="327" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O327" s="15"/>
+    </row>
+    <row r="328" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O328" s="15"/>
+    </row>
+    <row r="329" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O329" s="15"/>
+    </row>
+    <row r="330" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O330" s="15"/>
+    </row>
+    <row r="331" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O331" s="15"/>
+    </row>
+    <row r="332" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O332" s="15"/>
+    </row>
+    <row r="333" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O333" s="15"/>
+    </row>
+    <row r="334" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O334" s="15"/>
+    </row>
+    <row r="335" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O335" s="15"/>
+    </row>
+    <row r="336" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O336" s="15"/>
+    </row>
+    <row r="337" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O337" s="15"/>
+    </row>
+    <row r="338" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O338" s="15"/>
+    </row>
+    <row r="339" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O339" s="15"/>
+    </row>
+    <row r="340" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O340" s="15"/>
+    </row>
+    <row r="341" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O341" s="15"/>
+    </row>
+    <row r="342" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O342" s="15"/>
+    </row>
+    <row r="343" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O343" s="15"/>
+    </row>
+    <row r="344" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O344" s="15"/>
+    </row>
+    <row r="345" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O345" s="15"/>
+    </row>
+    <row r="346" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O346" s="15"/>
+    </row>
+    <row r="347" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O347" s="15"/>
+    </row>
+    <row r="348" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O348" s="15"/>
+    </row>
+    <row r="349" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O349" s="15"/>
+    </row>
+    <row r="350" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O350" s="15"/>
+    </row>
+    <row r="351" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O351" s="15"/>
+    </row>
+    <row r="352" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O352" s="15"/>
+    </row>
+    <row r="353" spans="15:15" x14ac:dyDescent="0.2">
+      <c r="O353" s="15"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>